<commit_message>
Updated Capital Budgeting spreadsheet
</commit_message>
<xml_diff>
--- a/fin_math/code/Capital Budgeting.xlsx
+++ b/fin_math/code/Capital Budgeting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfrat\Documents\_Work Related\_My Books\Financial Math with Python\CodeForBook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfrat\Documents\_Work Related\_My Books\Financial Math with Python\Review\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B55E15-58D4-4396-BE42-7C46F9E2182B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584ACDF3-16B0-4952-9E82-28B10B7F65E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="2790" windowWidth="23610" windowHeight="10500" firstSheet="2" activeTab="9" xr2:uid="{EAB1697F-5FC0-4B8A-A2CE-1FD59A4F4BBF}"/>
+    <workbookView xWindow="8325" yWindow="2310" windowWidth="14820" windowHeight="10920" xr2:uid="{EAB1697F-5FC0-4B8A-A2CE-1FD59A4F4BBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Acme Furniture" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>Rate of Return</t>
   </si>
@@ -171,6 +171,16 @@
   </si>
   <si>
     <t>Cost of Captial</t>
+  </si>
+  <si>
+    <t>Loan Example</t>
+  </si>
+  <si>
+    <t>Semi-annual 
+Cost of Captial</t>
+  </si>
+  <si>
+    <t>Semi-annual loan payment</t>
   </si>
 </sst>
 </file>
@@ -183,8 +193,8 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -342,34 +352,34 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -686,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650526AA-C8A1-4DA1-B4FF-57A6CB9267C3}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,105 +875,135 @@
         <v>7.7149201246496935E-2</v>
       </c>
     </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="20"/>
+    </row>
     <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B20" s="8">
         <v>-225000</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C20" s="8">
+        <f>C1-$B$21</f>
         <v>14931</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D20" s="8">
+        <f>D1-$B$21</f>
         <v>16931</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E20" s="8">
+        <f t="shared" ref="E20:N20" si="0">E1-$B$21</f>
         <v>18931</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
         <v>20931</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G20" s="8">
+        <f t="shared" si="0"/>
         <v>22931</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H20" s="8">
+        <f t="shared" si="0"/>
         <v>24931</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I20" s="8">
+        <f t="shared" si="0"/>
         <v>26931</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J20" s="8">
+        <f t="shared" si="0"/>
         <v>28931</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K20" s="8">
+        <f t="shared" si="0"/>
         <v>30931</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L20" s="8">
+        <f t="shared" si="0"/>
         <v>32931</v>
       </c>
-      <c r="M19" s="8">
+      <c r="M20" s="8">
+        <f>M1</f>
         <v>41000</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N20" s="8">
+        <f>N1</f>
         <v>44000</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="8">
+        <v>5069</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <f>NPV(0.02,B19:N19)</f>
-        <v>53625.158633028324</v>
-      </c>
-      <c r="B22" s="5">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <f>NPV(0.03,B19:N19)</f>
-        <v>34429.150303085931</v>
-      </c>
-      <c r="B23" s="5">
-        <v>0.03</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <f>NPV(0.04,B19:N19)</f>
-        <v>17289.978665402687</v>
+        <f>NPV(0.02,B20:N20)</f>
+        <v>53625.158633028324</v>
       </c>
       <c r="B24" s="5">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <f>NPV(0.05,B19:N19)</f>
-        <v>1971.444982003512</v>
+        <f>NPV(0.03,B20:N20)</f>
+        <v>34429.150303085931</v>
       </c>
       <c r="B25" s="5">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <f>NPV(0.06,B19:N19)</f>
+        <f>NPV(0.04,B20:N20)</f>
+        <v>17289.978665402687</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <f>NPV(0.05,B20:N20)</f>
+        <v>1971.444982003512</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <f>NPV(0.06,B20:N20)</f>
         <v>-11732.978259212809</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B28" s="5">
         <v>0.06</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -977,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0970F7-E0AC-495F-9A2C-6C9328FCD69A}">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,65 +1102,65 @@
       <c r="B2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="41">
+      <c r="C2" s="42"/>
+      <c r="D2" s="40">
         <v>20000</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="40">
         <v>22000</v>
       </c>
-      <c r="F2" s="41">
+      <c r="F2" s="40">
         <v>24000</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="40">
         <v>26000</v>
       </c>
-      <c r="H2" s="41">
+      <c r="H2" s="40">
         <v>28000</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2" s="40">
         <v>30000</v>
       </c>
-      <c r="J2" s="41">
+      <c r="J2" s="40">
         <v>32000</v>
       </c>
-      <c r="K2" s="41">
+      <c r="K2" s="40">
         <v>34000</v>
       </c>
-      <c r="L2" s="41">
+      <c r="L2" s="40">
         <v>36000</v>
       </c>
-      <c r="M2" s="41">
+      <c r="M2" s="40">
         <v>38000</v>
       </c>
-      <c r="N2" s="41">
+      <c r="N2" s="40">
         <v>41000</v>
       </c>
-      <c r="O2" s="41">
+      <c r="O2" s="40">
         <v>44000</v>
       </c>
-      <c r="P2" s="43">
+      <c r="P2" s="42">
         <v>0</v>
       </c>
-      <c r="Q2" s="43">
+      <c r="Q2" s="42">
         <v>0</v>
       </c>
-      <c r="R2" s="43">
+      <c r="R2" s="42">
         <v>0</v>
       </c>
-      <c r="S2" s="43">
+      <c r="S2" s="42">
         <v>0</v>
       </c>
-      <c r="T2" s="43">
+      <c r="T2" s="42">
         <v>0</v>
       </c>
-      <c r="U2" s="43">
+      <c r="U2" s="42">
         <v>0</v>
       </c>
-      <c r="V2" s="43">
+      <c r="V2" s="42">
         <v>0</v>
       </c>
-      <c r="W2" s="43">
+      <c r="W2" s="42">
         <v>0</v>
       </c>
     </row>
@@ -1128,67 +1168,67 @@
       <c r="B3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="40">
         <v>-225000</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="42">
         <v>-2566</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="42">
         <v>-2566</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <v>-2566</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="42">
         <v>-2566</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="42">
         <v>-2566</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="42">
         <v>-2566</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="42">
         <v>-2566</v>
       </c>
-      <c r="K3" s="43">
+      <c r="K3" s="42">
         <v>-2566</v>
       </c>
-      <c r="L3" s="43">
+      <c r="L3" s="42">
         <v>-2566</v>
       </c>
-      <c r="M3" s="43">
+      <c r="M3" s="42">
         <v>-2566</v>
       </c>
-      <c r="N3" s="43">
+      <c r="N3" s="42">
         <v>-2566</v>
       </c>
-      <c r="O3" s="43">
+      <c r="O3" s="42">
         <v>-2566</v>
       </c>
-      <c r="P3" s="43">
+      <c r="P3" s="42">
         <v>-2566</v>
       </c>
-      <c r="Q3" s="43">
+      <c r="Q3" s="42">
         <v>-2566</v>
       </c>
-      <c r="R3" s="43">
+      <c r="R3" s="42">
         <v>-2566</v>
       </c>
-      <c r="S3" s="43">
+      <c r="S3" s="42">
         <v>-2566</v>
       </c>
-      <c r="T3" s="43">
+      <c r="T3" s="42">
         <v>-2566</v>
       </c>
-      <c r="U3" s="43">
+      <c r="U3" s="42">
         <v>-2566</v>
       </c>
-      <c r="V3" s="43">
+      <c r="V3" s="42">
         <v>-2566</v>
       </c>
-      <c r="W3" s="43">
+      <c r="W3" s="42">
         <v>-2566</v>
       </c>
     </row>
@@ -1196,101 +1236,101 @@
       <c r="B4" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="42">
         <f>SUM(C2:C3)</f>
         <v>-225000</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="42">
         <f t="shared" ref="D4:W4" si="0">SUM(D2:D3)</f>
         <v>17434</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="42">
         <f t="shared" si="0"/>
         <v>19434</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="42">
         <f t="shared" si="0"/>
         <v>21434</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="42">
         <f t="shared" si="0"/>
         <v>23434</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="42">
         <f t="shared" si="0"/>
         <v>25434</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="42">
         <f t="shared" si="0"/>
         <v>27434</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <f t="shared" si="0"/>
         <v>29434</v>
       </c>
-      <c r="K4" s="43">
+      <c r="K4" s="42">
         <f t="shared" si="0"/>
         <v>31434</v>
       </c>
-      <c r="L4" s="43">
+      <c r="L4" s="42">
         <f t="shared" si="0"/>
         <v>33434</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="42">
         <f t="shared" si="0"/>
         <v>35434</v>
       </c>
-      <c r="N4" s="43">
+      <c r="N4" s="42">
         <f t="shared" si="0"/>
         <v>38434</v>
       </c>
-      <c r="O4" s="43">
+      <c r="O4" s="42">
         <f t="shared" si="0"/>
         <v>41434</v>
       </c>
-      <c r="P4" s="43">
+      <c r="P4" s="42">
         <f t="shared" si="0"/>
         <v>-2566</v>
       </c>
-      <c r="Q4" s="43">
+      <c r="Q4" s="42">
         <f t="shared" si="0"/>
         <v>-2566</v>
       </c>
-      <c r="R4" s="43">
+      <c r="R4" s="42">
         <f t="shared" si="0"/>
         <v>-2566</v>
       </c>
-      <c r="S4" s="43">
+      <c r="S4" s="42">
         <f t="shared" si="0"/>
         <v>-2566</v>
       </c>
-      <c r="T4" s="43">
+      <c r="T4" s="42">
         <f t="shared" si="0"/>
         <v>-2566</v>
       </c>
-      <c r="U4" s="43">
+      <c r="U4" s="42">
         <f t="shared" si="0"/>
         <v>-2566</v>
       </c>
-      <c r="V4" s="43">
+      <c r="V4" s="42">
         <f t="shared" si="0"/>
         <v>-2566</v>
       </c>
-      <c r="W4" s="43">
+      <c r="W4" s="42">
         <f t="shared" si="0"/>
         <v>-2566</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="44">
+      <c r="A9" s="43">
         <f>NPV(B9,$C$4:$W$4)</f>
         <v>57130.007098131922</v>
       </c>
@@ -1299,7 +1339,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="44">
+      <c r="A10" s="43">
         <f t="shared" ref="A10:A21" si="1">NPV(B10,$C$4:$W$4)</f>
         <v>48010.025661039232</v>
       </c>
@@ -1308,7 +1348,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="44">
+      <c r="A11" s="43">
         <f t="shared" si="1"/>
         <v>39345.652912491612</v>
       </c>
@@ -1317,7 +1357,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="44">
+      <c r="A12" s="43">
         <f t="shared" si="1"/>
         <v>31113.472319763805</v>
       </c>
@@ -1326,7 +1366,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="44">
+      <c r="A13" s="43">
         <f t="shared" si="1"/>
         <v>23291.27991959835</v>
       </c>
@@ -1335,7 +1375,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
+      <c r="A14" s="43">
         <f t="shared" si="1"/>
         <v>15858.028207577408</v>
       </c>
@@ -1344,7 +1384,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="44">
+      <c r="A15" s="43">
         <f t="shared" si="1"/>
         <v>8793.7712839846172</v>
       </c>
@@ -1353,7 +1393,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
+      <c r="A16" s="43">
         <f t="shared" si="1"/>
         <v>2079.6114765904472</v>
       </c>
@@ -1362,7 +1402,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="44">
+      <c r="A17" s="43">
         <f t="shared" si="1"/>
         <v>-4302.3523943234795</v>
       </c>
@@ -1371,7 +1411,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
+      <c r="A18" s="43">
         <f t="shared" si="1"/>
         <v>-10369.074989237455</v>
       </c>
@@ -1380,7 +1420,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="44">
+      <c r="A19" s="43">
         <f t="shared" si="1"/>
         <v>-16136.612579563285</v>
       </c>
@@ -1389,7 +1429,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="44">
+      <c r="A20" s="43">
         <f t="shared" si="1"/>
         <v>-21620.169284695137</v>
       </c>
@@ -1398,7 +1438,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="44">
+      <c r="A21" s="43">
         <f t="shared" si="1"/>
         <v>-26834.141391715682</v>
       </c>
@@ -2386,7 +2426,7 @@
       <c r="C20" s="17"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="39" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="21"/>
@@ -2416,7 +2456,7 @@
       <c r="B24" s="21"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="39" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="21"/>
@@ -2453,7 +2493,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,15 +2579,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="37"/>
-    <col min="2" max="2" width="10.7109375" style="37" customWidth="1"/>
-    <col min="3" max="3" width="15" style="37" customWidth="1"/>
-    <col min="4" max="9" width="9.85546875" style="37" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="37"/>
+    <col min="1" max="1" width="9.140625" style="36"/>
+    <col min="2" max="2" width="10.7109375" style="36" customWidth="1"/>
+    <col min="3" max="3" width="15" style="36" customWidth="1"/>
+    <col min="4" max="9" width="9.85546875" style="36" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>30</v>
       </c>
       <c r="D1" s="5">
@@ -2570,25 +2610,25 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="38">
         <v>-25000</v>
       </c>
-      <c r="E2" s="39">
+      <c r="E2" s="38">
         <v>-5000</v>
       </c>
-      <c r="F2" s="39">
+      <c r="F2" s="38">
         <v>5000</v>
       </c>
-      <c r="G2" s="39">
+      <c r="G2" s="38">
         <v>20000</v>
       </c>
-      <c r="H2" s="39">
+      <c r="H2" s="38">
         <v>20000</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="38">
         <v>20000</v>
       </c>
     </row>
@@ -2620,7 +2660,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,7 +2867,7 @@
       <c r="A9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="44">
         <f>B7/B8</f>
         <v>1.1623509000234862</v>
       </c>
@@ -3022,7 +3062,7 @@
       <c r="A19" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="36">
+      <c r="B19" s="35">
         <f>B17/B18</f>
         <v>1.1618446436104117</v>
       </c>
@@ -3040,7 +3080,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,28 +3128,28 @@
       <c r="C2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="41">
+      <c r="D2" s="40">
         <v>-70000</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="40">
         <v>5000</v>
       </c>
-      <c r="F2" s="41">
+      <c r="F2" s="40">
         <v>7500</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="40">
         <v>10000</v>
       </c>
-      <c r="H2" s="41">
+      <c r="H2" s="40">
         <v>12500</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2" s="40">
         <v>15000</v>
       </c>
-      <c r="J2" s="41">
+      <c r="J2" s="40">
         <v>17500</v>
       </c>
-      <c r="K2" s="41">
+      <c r="K2" s="40">
         <v>20000</v>
       </c>
     </row>
@@ -3122,7 +3162,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="42">
+      <c r="A5" s="41">
         <f>NPV(B5,$D$2:$K$2)</f>
         <v>9430.0811003782946</v>
       </c>
@@ -3131,7 +3171,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="42">
+      <c r="A6" s="41">
         <f t="shared" ref="A6:A10" si="0">NPV(B6,$D$2:$K$2)</f>
         <v>5862.4072112749327</v>
       </c>
@@ -3140,7 +3180,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="42">
+      <c r="A7" s="41">
         <f t="shared" si="0"/>
         <v>2571.7759092454239</v>
       </c>
@@ -3149,7 +3189,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="42">
+      <c r="A8" s="41">
         <f t="shared" si="0"/>
         <v>-464.69398921551533</v>
       </c>
@@ -3158,7 +3198,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="42">
+      <c r="A9" s="41">
         <f t="shared" si="0"/>
         <v>-3267.790211214663</v>
       </c>
@@ -3167,7 +3207,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="42">
+      <c r="A10" s="41">
         <f t="shared" si="0"/>
         <v>-5856.41773406621</v>
       </c>

</xml_diff>